<commit_message>
Update to trade logic
</commit_message>
<xml_diff>
--- a/user_team.xlsx
+++ b/user_team.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afloy\OneDrive\Desktop\FantasyPremML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF4BDA2-A5BC-431E-A4DE-21B5C5721EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4434925B-3CC6-4242-BC49-DFD2C6266A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="10455" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>Player</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Free Transfers</t>
+  </si>
+  <si>
+    <t>Injured</t>
   </si>
 </sst>
 </file>
@@ -202,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -212,6 +215,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,16 +499,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -535,8 +542,11 @@
       <c r="K1" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>430</v>
       </c>
@@ -566,10 +576,13 @@
         <v>0.2</v>
       </c>
       <c r="K2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>381</v>
       </c>
@@ -595,8 +608,11 @@
       <c r="I3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -622,8 +638,11 @@
       <c r="I4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>507</v>
       </c>
@@ -649,8 +668,11 @@
       <c r="I5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>38</v>
       </c>
@@ -675,8 +697,11 @@
       <c r="I6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="L6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>427</v>
       </c>
@@ -701,8 +726,11 @@
       <c r="I7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>382</v>
       </c>
@@ -727,8 +755,11 @@
       <c r="I8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="L8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>241</v>
       </c>
@@ -753,8 +784,11 @@
       <c r="I9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="L9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>666</v>
       </c>
@@ -779,8 +813,11 @@
       <c r="I10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="L10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>470</v>
       </c>
@@ -805,8 +842,11 @@
       <c r="I11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>287</v>
       </c>
@@ -829,10 +869,13 @@
         <v>0</v>
       </c>
       <c r="I12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="L12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>43</v>
       </c>
@@ -857,8 +900,11 @@
       <c r="I13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>211</v>
       </c>
@@ -883,8 +929,11 @@
       <c r="I14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>467</v>
       </c>
@@ -907,6 +956,9 @@
         <v>0</v>
       </c>
       <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>